<commit_message>
Fixed typo in age column header
</commit_message>
<xml_diff>
--- a/templates/narvarokort_sthlm.xlsx
+++ b/templates/narvarokort_sthlm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobbe/proj/github/stgscout/skojjt/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF1A100-A55A-8B46-A9F6-D20276B0209C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C434C749-8603-CF4B-8D4C-212FC484DA2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7180" yWindow="1060" windowWidth="28080" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,9 +213,6 @@
     <t>10-12</t>
   </si>
   <si>
-    <t>13-15</t>
-  </si>
-  <si>
     <t>17-20</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>Scoutkår X</t>
+  </si>
+  <si>
+    <t>13-16</t>
   </si>
 </sst>
 </file>
@@ -1584,52 +1584,25 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
@@ -1670,22 +1643,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2224,7 +2224,7 @@
   <dimension ref="A1:CU149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="AK14" sqref="AK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2242,25 +2242,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:99" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="123" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="124"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="116" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="117"/>
       <c r="G1" s="24" t="s">
         <v>8</v>
       </c>
       <c r="AI1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="114">
+      <c r="AJ1" s="125">
         <v>2019</v>
       </c>
-      <c r="AK1" s="115"/>
+      <c r="AK1" s="126"/>
     </row>
     <row r="2" spans="1:99" s="1" customFormat="1" ht="11" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -2273,7 +2273,7 @@
     </row>
     <row r="3" spans="1:99" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
@@ -2358,74 +2358,74 @@
         <v>11</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="129" t="s">
+      <c r="C4" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="130"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="125" t="s">
+      <c r="D4" s="123"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="116"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
-      <c r="L4" s="116"/>
-      <c r="M4" s="116"/>
-      <c r="N4" s="116"/>
-      <c r="O4" s="116"/>
-      <c r="P4" s="116"/>
-      <c r="Q4" s="116"/>
-      <c r="R4" s="116"/>
-      <c r="S4" s="118"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
-      <c r="V4" s="118"/>
-      <c r="W4" s="116"/>
-      <c r="X4" s="116"/>
-      <c r="Y4" s="116"/>
-      <c r="Z4" s="116"/>
-      <c r="AA4" s="116"/>
-      <c r="AB4" s="117"/>
-      <c r="AC4" s="111"/>
-      <c r="AD4" s="111"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
+      <c r="K4" s="110"/>
+      <c r="L4" s="110"/>
+      <c r="M4" s="110"/>
+      <c r="N4" s="110"/>
+      <c r="O4" s="110"/>
+      <c r="P4" s="110"/>
+      <c r="Q4" s="110"/>
+      <c r="R4" s="110"/>
+      <c r="S4" s="111"/>
+      <c r="T4" s="111"/>
+      <c r="U4" s="111"/>
+      <c r="V4" s="111"/>
+      <c r="W4" s="110"/>
+      <c r="X4" s="110"/>
+      <c r="Y4" s="110"/>
+      <c r="Z4" s="110"/>
+      <c r="AA4" s="110"/>
+      <c r="AB4" s="127"/>
+      <c r="AC4" s="135"/>
+      <c r="AD4" s="135"/>
     </row>
     <row r="5" spans="1:99" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="97"/>
-      <c r="C5" s="126" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="127"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="119"/>
-      <c r="T5" s="119"/>
-      <c r="U5" s="119"/>
-      <c r="V5" s="119"/>
-      <c r="W5" s="116"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="116"/>
-      <c r="Z5" s="116"/>
-      <c r="AA5" s="116"/>
-      <c r="AB5" s="117"/>
-      <c r="AC5" s="112"/>
-      <c r="AD5" s="112"/>
+      <c r="C5" s="119" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="120"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="110"/>
+      <c r="L5" s="110"/>
+      <c r="M5" s="110"/>
+      <c r="N5" s="110"/>
+      <c r="O5" s="110"/>
+      <c r="P5" s="110"/>
+      <c r="Q5" s="110"/>
+      <c r="R5" s="110"/>
+      <c r="S5" s="112"/>
+      <c r="T5" s="112"/>
+      <c r="U5" s="112"/>
+      <c r="V5" s="112"/>
+      <c r="W5" s="110"/>
+      <c r="X5" s="110"/>
+      <c r="Y5" s="110"/>
+      <c r="Z5" s="110"/>
+      <c r="AA5" s="110"/>
+      <c r="AB5" s="127"/>
+      <c r="AC5" s="136"/>
+      <c r="AD5" s="136"/>
     </row>
     <row r="6" spans="1:99" s="1" customFormat="1" ht="10" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
@@ -2435,65 +2435,65 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="116"/>
-      <c r="M6" s="116"/>
-      <c r="N6" s="116"/>
-      <c r="O6" s="116"/>
-      <c r="P6" s="116"/>
-      <c r="Q6" s="116"/>
-      <c r="R6" s="116"/>
-      <c r="S6" s="119"/>
-      <c r="T6" s="119"/>
-      <c r="U6" s="119"/>
-      <c r="V6" s="119"/>
-      <c r="W6" s="116"/>
-      <c r="X6" s="116"/>
-      <c r="Y6" s="116"/>
-      <c r="Z6" s="116"/>
-      <c r="AA6" s="116"/>
-      <c r="AB6" s="117"/>
-      <c r="AC6" s="112"/>
-      <c r="AD6" s="112"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="110"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="110"/>
+      <c r="M6" s="110"/>
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="110"/>
+      <c r="Q6" s="110"/>
+      <c r="R6" s="110"/>
+      <c r="S6" s="112"/>
+      <c r="T6" s="112"/>
+      <c r="U6" s="112"/>
+      <c r="V6" s="112"/>
+      <c r="W6" s="110"/>
+      <c r="X6" s="110"/>
+      <c r="Y6" s="110"/>
+      <c r="Z6" s="110"/>
+      <c r="AA6" s="110"/>
+      <c r="AB6" s="127"/>
+      <c r="AC6" s="136"/>
+      <c r="AD6" s="136"/>
     </row>
     <row r="7" spans="1:99" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
-      <c r="L7" s="116"/>
-      <c r="M7" s="116"/>
-      <c r="N7" s="116"/>
-      <c r="O7" s="116"/>
-      <c r="P7" s="116"/>
-      <c r="Q7" s="116"/>
-      <c r="R7" s="116"/>
-      <c r="S7" s="119"/>
-      <c r="T7" s="119"/>
-      <c r="U7" s="119"/>
-      <c r="V7" s="119"/>
-      <c r="W7" s="116"/>
-      <c r="X7" s="116"/>
-      <c r="Y7" s="116"/>
-      <c r="Z7" s="116"/>
-      <c r="AA7" s="116"/>
-      <c r="AB7" s="117"/>
-      <c r="AC7" s="112"/>
-      <c r="AD7" s="112"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
+      <c r="K7" s="110"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="110"/>
+      <c r="N7" s="110"/>
+      <c r="O7" s="110"/>
+      <c r="P7" s="110"/>
+      <c r="Q7" s="110"/>
+      <c r="R7" s="110"/>
+      <c r="S7" s="112"/>
+      <c r="T7" s="112"/>
+      <c r="U7" s="112"/>
+      <c r="V7" s="112"/>
+      <c r="W7" s="110"/>
+      <c r="X7" s="110"/>
+      <c r="Y7" s="110"/>
+      <c r="Z7" s="110"/>
+      <c r="AA7" s="110"/>
+      <c r="AB7" s="127"/>
+      <c r="AC7" s="136"/>
+      <c r="AD7" s="136"/>
     </row>
     <row r="8" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
@@ -2503,31 +2503,31 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="116"/>
-      <c r="M8" s="116"/>
-      <c r="N8" s="116"/>
-      <c r="O8" s="116"/>
-      <c r="P8" s="116"/>
-      <c r="Q8" s="116"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="119"/>
-      <c r="T8" s="119"/>
-      <c r="U8" s="119"/>
-      <c r="V8" s="119"/>
-      <c r="W8" s="116"/>
-      <c r="X8" s="116"/>
-      <c r="Y8" s="116"/>
-      <c r="Z8" s="116"/>
-      <c r="AA8" s="116"/>
-      <c r="AB8" s="117"/>
-      <c r="AC8" s="112"/>
-      <c r="AD8" s="112"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
+      <c r="K8" s="110"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="110"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="110"/>
+      <c r="S8" s="112"/>
+      <c r="T8" s="112"/>
+      <c r="U8" s="112"/>
+      <c r="V8" s="112"/>
+      <c r="W8" s="110"/>
+      <c r="X8" s="110"/>
+      <c r="Y8" s="110"/>
+      <c r="Z8" s="110"/>
+      <c r="AA8" s="110"/>
+      <c r="AB8" s="127"/>
+      <c r="AC8" s="136"/>
+      <c r="AD8" s="136"/>
     </row>
     <row r="9" spans="1:99" s="1" customFormat="1" ht="10" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
@@ -2537,38 +2537,38 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="125"/>
-      <c r="G9" s="116"/>
-      <c r="H9" s="116"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
-      <c r="M9" s="116"/>
-      <c r="N9" s="116"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="116"/>
-      <c r="Q9" s="116"/>
-      <c r="R9" s="116"/>
-      <c r="S9" s="120"/>
-      <c r="T9" s="120"/>
-      <c r="U9" s="120"/>
-      <c r="V9" s="120"/>
-      <c r="W9" s="116"/>
-      <c r="X9" s="116"/>
-      <c r="Y9" s="116"/>
-      <c r="Z9" s="116"/>
-      <c r="AA9" s="116"/>
-      <c r="AB9" s="117"/>
-      <c r="AC9" s="113"/>
-      <c r="AD9" s="113"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
+      <c r="K9" s="110"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="110"/>
+      <c r="N9" s="110"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="110"/>
+      <c r="Q9" s="110"/>
+      <c r="R9" s="110"/>
+      <c r="S9" s="113"/>
+      <c r="T9" s="113"/>
+      <c r="U9" s="113"/>
+      <c r="V9" s="113"/>
+      <c r="W9" s="110"/>
+      <c r="X9" s="110"/>
+      <c r="Y9" s="110"/>
+      <c r="Z9" s="110"/>
+      <c r="AA9" s="110"/>
+      <c r="AB9" s="127"/>
+      <c r="AC9" s="137"/>
+      <c r="AD9" s="137"/>
     </row>
     <row r="10" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="132"/>
-      <c r="B10" s="133"/>
-      <c r="C10" s="133"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="134"/>
+      <c r="A10" s="104"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="106"/>
       <c r="F10" s="14" t="s">
         <v>18</v>
       </c>
@@ -2598,11 +2598,11 @@
       <c r="AD10" s="65"/>
     </row>
     <row r="11" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="132"/>
-      <c r="B11" s="133"/>
-      <c r="C11" s="133"/>
-      <c r="D11" s="133"/>
-      <c r="E11" s="134"/>
+      <c r="A11" s="104"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="106"/>
       <c r="F11" s="14" t="s">
         <v>19</v>
       </c>
@@ -2632,11 +2632,11 @@
       <c r="AD11" s="65"/>
     </row>
     <row r="12" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="135"/>
-      <c r="B12" s="136"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="137"/>
+      <c r="A12" s="107"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="109"/>
       <c r="F12" s="14" t="s">
         <v>20</v>
       </c>
@@ -2664,16 +2664,16 @@
       <c r="AB12" s="31"/>
       <c r="AC12" s="31"/>
       <c r="AD12" s="31"/>
-      <c r="AE12" s="108" t="s">
+      <c r="AE12" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="AF12" s="109"/>
-      <c r="AG12" s="109"/>
-      <c r="AH12" s="109"/>
-      <c r="AI12" s="109"/>
-      <c r="AJ12" s="109"/>
-      <c r="AK12" s="109"/>
-      <c r="AL12" s="110"/>
+      <c r="AF12" s="133"/>
+      <c r="AG12" s="133"/>
+      <c r="AH12" s="133"/>
+      <c r="AI12" s="133"/>
+      <c r="AJ12" s="133"/>
+      <c r="AK12" s="133"/>
+      <c r="AL12" s="134"/>
       <c r="AM12" s="66"/>
     </row>
     <row r="13" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2711,18 +2711,18 @@
       <c r="AB13" s="31"/>
       <c r="AC13" s="31"/>
       <c r="AD13" s="31"/>
-      <c r="AE13" s="104" t="s">
+      <c r="AE13" s="128" t="s">
         <v>24</v>
       </c>
-      <c r="AF13" s="105"/>
-      <c r="AG13" s="105"/>
-      <c r="AH13" s="105"/>
-      <c r="AI13" s="106" t="s">
+      <c r="AF13" s="129"/>
+      <c r="AG13" s="129"/>
+      <c r="AH13" s="129"/>
+      <c r="AI13" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="AJ13" s="105"/>
-      <c r="AK13" s="105"/>
-      <c r="AL13" s="107"/>
+      <c r="AJ13" s="129"/>
+      <c r="AK13" s="129"/>
+      <c r="AL13" s="131"/>
       <c r="AM13" s="66"/>
     </row>
     <row r="14" spans="1:99" ht="14" thickBot="1" x14ac:dyDescent="0.2">
@@ -2773,10 +2773,10 @@
         <v>31</v>
       </c>
       <c r="AG14" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH14" s="27" t="s">
         <v>32</v>
-      </c>
-      <c r="AH14" s="27" t="s">
-        <v>33</v>
       </c>
       <c r="AI14" s="28" t="s">
         <v>30</v>
@@ -2785,10 +2785,10 @@
         <v>31</v>
       </c>
       <c r="AK14" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL14" s="45" t="s">
         <v>32</v>
-      </c>
-      <c r="AL14" s="45" t="s">
-        <v>33</v>
       </c>
       <c r="AM14" s="66"/>
     </row>
@@ -8810,6 +8810,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="AE13:AH13"/>
+    <mergeCell ref="AI13:AL13"/>
+    <mergeCell ref="AE12:AL12"/>
+    <mergeCell ref="AD4:AD9"/>
+    <mergeCell ref="AC4:AC9"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="Q4:Q9"/>
+    <mergeCell ref="R4:R9"/>
+    <mergeCell ref="AB4:AB9"/>
+    <mergeCell ref="AA4:AA9"/>
+    <mergeCell ref="Z4:Z9"/>
+    <mergeCell ref="T4:T9"/>
+    <mergeCell ref="W4:W9"/>
+    <mergeCell ref="X4:X9"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="G4:G9"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C4:E4"/>
     <mergeCell ref="A10:E12"/>
     <mergeCell ref="Y4:Y9"/>
     <mergeCell ref="V4:V9"/>
@@ -8824,26 +8844,6 @@
     <mergeCell ref="H4:H9"/>
     <mergeCell ref="L4:L9"/>
     <mergeCell ref="K4:K9"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F4:F9"/>
-    <mergeCell ref="G4:G9"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="Q4:Q9"/>
-    <mergeCell ref="R4:R9"/>
-    <mergeCell ref="AB4:AB9"/>
-    <mergeCell ref="AA4:AA9"/>
-    <mergeCell ref="Z4:Z9"/>
-    <mergeCell ref="T4:T9"/>
-    <mergeCell ref="W4:W9"/>
-    <mergeCell ref="X4:X9"/>
-    <mergeCell ref="AE13:AH13"/>
-    <mergeCell ref="AI13:AL13"/>
-    <mergeCell ref="AE12:AL12"/>
-    <mergeCell ref="AD4:AD9"/>
-    <mergeCell ref="AC4:AC9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Uppdaterade mallar för Stockholm utan bilder (funkar inte med eller utab PIL/Pillow).
</commit_message>
<xml_diff>
--- a/templates/narvarokort_sthlm.xlsx
+++ b/templates/narvarokort_sthlm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobbe/proj/github/stgscout/skojjt/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\skojjt\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C434C749-8603-CF4B-8D4C-212FC484DA2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F3FC91-E5E1-43F1-91CA-EB04972972E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7180" yWindow="1060" windowWidth="28080" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Närvarokort" sheetId="1" r:id="rId1"/>
@@ -1584,25 +1584,52 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment textRotation="90"/>
       <protection locked="0"/>
     </xf>
@@ -1643,49 +1670,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1817,85 +1817,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1034" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E393D93F-BEB8-E54F-89F2-1DE3F52DB5FA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="12941300" y="457200"/>
-          <a:ext cx="1295400" cy="1384300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2224,45 +2145,45 @@
   <dimension ref="A1:CU149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="AK14" sqref="AK14"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="3.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" customWidth="1"/>
-    <col min="7" max="30" width="3.33203125" customWidth="1"/>
-    <col min="31" max="37" width="4.33203125" customWidth="1"/>
-    <col min="38" max="38" width="4.6640625" customWidth="1"/>
-    <col min="39" max="39" width="1.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="3.6328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="7.1796875" customWidth="1"/>
+    <col min="7" max="30" width="3.36328125" customWidth="1"/>
+    <col min="31" max="37" width="4.36328125" customWidth="1"/>
+    <col min="38" max="38" width="4.6328125" customWidth="1"/>
+    <col min="39" max="39" width="1.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:99" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="116" t="s">
+      <c r="B1" s="121"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="117"/>
+      <c r="E1" s="124"/>
       <c r="G1" s="24" t="s">
         <v>8</v>
       </c>
       <c r="AI1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="125">
+      <c r="AJ1" s="114">
         <v>2019</v>
       </c>
-      <c r="AK1" s="126"/>
+      <c r="AK1" s="115"/>
     </row>
-    <row r="2" spans="1:99" s="1" customFormat="1" ht="11" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:99" s="1" customFormat="1" ht="8.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -2271,7 +2192,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:99" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:99" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
         <v>36</v>
       </c>
@@ -2353,81 +2274,81 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:99" s="1" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:99" s="1" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="122" t="s">
+      <c r="C4" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="123"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="118" t="s">
+      <c r="D4" s="130"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="110"/>
-      <c r="N4" s="110"/>
-      <c r="O4" s="110"/>
-      <c r="P4" s="110"/>
-      <c r="Q4" s="110"/>
-      <c r="R4" s="110"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="111"/>
-      <c r="W4" s="110"/>
-      <c r="X4" s="110"/>
-      <c r="Y4" s="110"/>
-      <c r="Z4" s="110"/>
-      <c r="AA4" s="110"/>
-      <c r="AB4" s="127"/>
-      <c r="AC4" s="135"/>
-      <c r="AD4" s="135"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
+      <c r="M4" s="116"/>
+      <c r="N4" s="116"/>
+      <c r="O4" s="116"/>
+      <c r="P4" s="116"/>
+      <c r="Q4" s="116"/>
+      <c r="R4" s="116"/>
+      <c r="S4" s="118"/>
+      <c r="T4" s="118"/>
+      <c r="U4" s="118"/>
+      <c r="V4" s="118"/>
+      <c r="W4" s="116"/>
+      <c r="X4" s="116"/>
+      <c r="Y4" s="116"/>
+      <c r="Z4" s="116"/>
+      <c r="AA4" s="116"/>
+      <c r="AB4" s="117"/>
+      <c r="AC4" s="111"/>
+      <c r="AD4" s="111"/>
     </row>
-    <row r="5" spans="1:99" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:99" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="97"/>
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-      <c r="L5" s="110"/>
-      <c r="M5" s="110"/>
-      <c r="N5" s="110"/>
-      <c r="O5" s="110"/>
-      <c r="P5" s="110"/>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="110"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="110"/>
-      <c r="Y5" s="110"/>
-      <c r="Z5" s="110"/>
-      <c r="AA5" s="110"/>
-      <c r="AB5" s="127"/>
-      <c r="AC5" s="136"/>
-      <c r="AD5" s="136"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="116"/>
+      <c r="R5" s="116"/>
+      <c r="S5" s="119"/>
+      <c r="T5" s="119"/>
+      <c r="U5" s="119"/>
+      <c r="V5" s="119"/>
+      <c r="W5" s="116"/>
+      <c r="X5" s="116"/>
+      <c r="Y5" s="116"/>
+      <c r="Z5" s="116"/>
+      <c r="AA5" s="116"/>
+      <c r="AB5" s="117"/>
+      <c r="AC5" s="112"/>
+      <c r="AD5" s="112"/>
     </row>
-    <row r="6" spans="1:99" s="1" customFormat="1" ht="10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:99" s="1" customFormat="1" ht="8" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -2435,33 +2356,33 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="110"/>
-      <c r="Q6" s="110"/>
-      <c r="R6" s="110"/>
-      <c r="S6" s="112"/>
-      <c r="T6" s="112"/>
-      <c r="U6" s="112"/>
-      <c r="V6" s="112"/>
-      <c r="W6" s="110"/>
-      <c r="X6" s="110"/>
-      <c r="Y6" s="110"/>
-      <c r="Z6" s="110"/>
-      <c r="AA6" s="110"/>
-      <c r="AB6" s="127"/>
-      <c r="AC6" s="136"/>
-      <c r="AD6" s="136"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="116"/>
+      <c r="K6" s="116"/>
+      <c r="L6" s="116"/>
+      <c r="M6" s="116"/>
+      <c r="N6" s="116"/>
+      <c r="O6" s="116"/>
+      <c r="P6" s="116"/>
+      <c r="Q6" s="116"/>
+      <c r="R6" s="116"/>
+      <c r="S6" s="119"/>
+      <c r="T6" s="119"/>
+      <c r="U6" s="119"/>
+      <c r="V6" s="119"/>
+      <c r="W6" s="116"/>
+      <c r="X6" s="116"/>
+      <c r="Y6" s="116"/>
+      <c r="Z6" s="116"/>
+      <c r="AA6" s="116"/>
+      <c r="AB6" s="117"/>
+      <c r="AC6" s="112"/>
+      <c r="AD6" s="112"/>
     </row>
-    <row r="7" spans="1:99" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:99" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
         <v>35</v>
       </c>
@@ -2469,33 +2390,33 @@
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="110"/>
-      <c r="N7" s="110"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
-      <c r="Q7" s="110"/>
-      <c r="R7" s="110"/>
-      <c r="S7" s="112"/>
-      <c r="T7" s="112"/>
-      <c r="U7" s="112"/>
-      <c r="V7" s="112"/>
-      <c r="W7" s="110"/>
-      <c r="X7" s="110"/>
-      <c r="Y7" s="110"/>
-      <c r="Z7" s="110"/>
-      <c r="AA7" s="110"/>
-      <c r="AB7" s="127"/>
-      <c r="AC7" s="136"/>
-      <c r="AD7" s="136"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="116"/>
+      <c r="M7" s="116"/>
+      <c r="N7" s="116"/>
+      <c r="O7" s="116"/>
+      <c r="P7" s="116"/>
+      <c r="Q7" s="116"/>
+      <c r="R7" s="116"/>
+      <c r="S7" s="119"/>
+      <c r="T7" s="119"/>
+      <c r="U7" s="119"/>
+      <c r="V7" s="119"/>
+      <c r="W7" s="116"/>
+      <c r="X7" s="116"/>
+      <c r="Y7" s="116"/>
+      <c r="Z7" s="116"/>
+      <c r="AA7" s="116"/>
+      <c r="AB7" s="117"/>
+      <c r="AC7" s="112"/>
+      <c r="AD7" s="112"/>
     </row>
-    <row r="8" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>16</v>
       </c>
@@ -2503,33 +2424,33 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="110"/>
-      <c r="H8" s="110"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="110"/>
-      <c r="K8" s="110"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="110"/>
-      <c r="N8" s="110"/>
-      <c r="O8" s="110"/>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="110"/>
-      <c r="R8" s="110"/>
-      <c r="S8" s="112"/>
-      <c r="T8" s="112"/>
-      <c r="U8" s="112"/>
-      <c r="V8" s="112"/>
-      <c r="W8" s="110"/>
-      <c r="X8" s="110"/>
-      <c r="Y8" s="110"/>
-      <c r="Z8" s="110"/>
-      <c r="AA8" s="110"/>
-      <c r="AB8" s="127"/>
-      <c r="AC8" s="136"/>
-      <c r="AD8" s="136"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="116"/>
+      <c r="K8" s="116"/>
+      <c r="L8" s="116"/>
+      <c r="M8" s="116"/>
+      <c r="N8" s="116"/>
+      <c r="O8" s="116"/>
+      <c r="P8" s="116"/>
+      <c r="Q8" s="116"/>
+      <c r="R8" s="116"/>
+      <c r="S8" s="119"/>
+      <c r="T8" s="119"/>
+      <c r="U8" s="119"/>
+      <c r="V8" s="119"/>
+      <c r="W8" s="116"/>
+      <c r="X8" s="116"/>
+      <c r="Y8" s="116"/>
+      <c r="Z8" s="116"/>
+      <c r="AA8" s="116"/>
+      <c r="AB8" s="117"/>
+      <c r="AC8" s="112"/>
+      <c r="AD8" s="112"/>
     </row>
-    <row r="9" spans="1:99" s="1" customFormat="1" ht="10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:99" s="1" customFormat="1" ht="8" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
@@ -2537,38 +2458,38 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="110"/>
-      <c r="N9" s="110"/>
-      <c r="O9" s="110"/>
-      <c r="P9" s="110"/>
-      <c r="Q9" s="110"/>
-      <c r="R9" s="110"/>
-      <c r="S9" s="113"/>
-      <c r="T9" s="113"/>
-      <c r="U9" s="113"/>
-      <c r="V9" s="113"/>
-      <c r="W9" s="110"/>
-      <c r="X9" s="110"/>
-      <c r="Y9" s="110"/>
-      <c r="Z9" s="110"/>
-      <c r="AA9" s="110"/>
-      <c r="AB9" s="127"/>
-      <c r="AC9" s="137"/>
-      <c r="AD9" s="137"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="116"/>
+      <c r="H9" s="116"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116"/>
+      <c r="M9" s="116"/>
+      <c r="N9" s="116"/>
+      <c r="O9" s="116"/>
+      <c r="P9" s="116"/>
+      <c r="Q9" s="116"/>
+      <c r="R9" s="116"/>
+      <c r="S9" s="120"/>
+      <c r="T9" s="120"/>
+      <c r="U9" s="120"/>
+      <c r="V9" s="120"/>
+      <c r="W9" s="116"/>
+      <c r="X9" s="116"/>
+      <c r="Y9" s="116"/>
+      <c r="Z9" s="116"/>
+      <c r="AA9" s="116"/>
+      <c r="AB9" s="117"/>
+      <c r="AC9" s="113"/>
+      <c r="AD9" s="113"/>
     </row>
-    <row r="10" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="104"/>
-      <c r="B10" s="105"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="106"/>
+    <row r="10" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="132"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="134"/>
       <c r="F10" s="14" t="s">
         <v>18</v>
       </c>
@@ -2597,12 +2518,12 @@
       <c r="AC10" s="65"/>
       <c r="AD10" s="65"/>
     </row>
-    <row r="11" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="104"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="106"/>
+    <row r="11" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="132"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="133"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="134"/>
       <c r="F11" s="14" t="s">
         <v>19</v>
       </c>
@@ -2631,12 +2552,12 @@
       <c r="AC11" s="65"/>
       <c r="AD11" s="65"/>
     </row>
-    <row r="12" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="107"/>
-      <c r="B12" s="108"/>
-      <c r="C12" s="108"/>
-      <c r="D12" s="108"/>
-      <c r="E12" s="109"/>
+    <row r="12" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="135"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="137"/>
       <c r="F12" s="14" t="s">
         <v>20</v>
       </c>
@@ -2664,19 +2585,19 @@
       <c r="AB12" s="31"/>
       <c r="AC12" s="31"/>
       <c r="AD12" s="31"/>
-      <c r="AE12" s="132" t="s">
+      <c r="AE12" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="AF12" s="133"/>
-      <c r="AG12" s="133"/>
-      <c r="AH12" s="133"/>
-      <c r="AI12" s="133"/>
-      <c r="AJ12" s="133"/>
-      <c r="AK12" s="133"/>
-      <c r="AL12" s="134"/>
+      <c r="AF12" s="109"/>
+      <c r="AG12" s="109"/>
+      <c r="AH12" s="109"/>
+      <c r="AI12" s="109"/>
+      <c r="AJ12" s="109"/>
+      <c r="AK12" s="109"/>
+      <c r="AL12" s="110"/>
       <c r="AM12" s="66"/>
     </row>
-    <row r="13" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="16" t="s">
         <v>22</v>
@@ -2711,21 +2632,21 @@
       <c r="AB13" s="31"/>
       <c r="AC13" s="31"/>
       <c r="AD13" s="31"/>
-      <c r="AE13" s="128" t="s">
+      <c r="AE13" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="AF13" s="129"/>
-      <c r="AG13" s="129"/>
-      <c r="AH13" s="129"/>
-      <c r="AI13" s="130" t="s">
+      <c r="AF13" s="105"/>
+      <c r="AG13" s="105"/>
+      <c r="AH13" s="105"/>
+      <c r="AI13" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="AJ13" s="129"/>
-      <c r="AK13" s="129"/>
-      <c r="AL13" s="131"/>
+      <c r="AJ13" s="105"/>
+      <c r="AK13" s="105"/>
+      <c r="AL13" s="107"/>
       <c r="AM13" s="66"/>
     </row>
-    <row r="14" spans="1:99" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:99" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="17" t="s">
         <v>26</v>
@@ -2792,7 +2713,7 @@
       </c>
       <c r="AM14" s="66"/>
     </row>
-    <row r="15" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>1</v>
       </c>
@@ -2862,7 +2783,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>2</v>
       </c>
@@ -2992,7 +2913,7 @@
       <c r="CT16" s="6"/>
       <c r="CU16" s="6"/>
     </row>
-    <row r="17" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>3</v>
       </c>
@@ -3122,7 +3043,7 @@
       <c r="CT17" s="6"/>
       <c r="CU17" s="6"/>
     </row>
-    <row r="18" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>4</v>
       </c>
@@ -3192,7 +3113,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>5</v>
       </c>
@@ -3262,7 +3183,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>6</v>
       </c>
@@ -3392,7 +3313,7 @@
       <c r="CT20" s="6"/>
       <c r="CU20" s="6"/>
     </row>
-    <row r="21" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>7</v>
       </c>
@@ -3522,7 +3443,7 @@
       <c r="CT21" s="6"/>
       <c r="CU21" s="6"/>
     </row>
-    <row r="22" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>8</v>
       </c>
@@ -3592,7 +3513,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>9</v>
       </c>
@@ -3662,7 +3583,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>10</v>
       </c>
@@ -3792,7 +3713,7 @@
       <c r="CT24" s="6"/>
       <c r="CU24" s="6"/>
     </row>
-    <row r="25" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>11</v>
       </c>
@@ -3922,7 +3843,7 @@
       <c r="CT25" s="6"/>
       <c r="CU25" s="6"/>
     </row>
-    <row r="26" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>12</v>
       </c>
@@ -4052,7 +3973,7 @@
       <c r="CT26" s="6"/>
       <c r="CU26" s="6"/>
     </row>
-    <row r="27" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>13</v>
       </c>
@@ -4182,7 +4103,7 @@
       <c r="CT27" s="6"/>
       <c r="CU27" s="6"/>
     </row>
-    <row r="28" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>15</v>
       </c>
@@ -4312,7 +4233,7 @@
       <c r="CT28" s="6"/>
       <c r="CU28" s="6"/>
     </row>
-    <row r="29" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>16</v>
       </c>
@@ -4442,7 +4363,7 @@
       <c r="CT29" s="6"/>
       <c r="CU29" s="6"/>
     </row>
-    <row r="30" spans="1:99" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:99" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>17</v>
       </c>
@@ -4512,7 +4433,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:99" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:99" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>18</v>
       </c>
@@ -4582,7 +4503,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>19</v>
       </c>
@@ -4652,7 +4573,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>20</v>
       </c>
@@ -4722,7 +4643,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:99" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:99" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>21</v>
       </c>
@@ -4792,7 +4713,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>22</v>
       </c>
@@ -4922,7 +4843,7 @@
       <c r="CT35" s="6"/>
       <c r="CU35" s="6"/>
     </row>
-    <row r="36" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
         <v>23</v>
       </c>
@@ -4992,7 +4913,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>24</v>
       </c>
@@ -5122,7 +5043,7 @@
       <c r="CT37" s="6"/>
       <c r="CU37" s="6"/>
     </row>
-    <row r="38" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>25</v>
       </c>
@@ -5252,7 +5173,7 @@
       <c r="CT38" s="6"/>
       <c r="CU38" s="6"/>
     </row>
-    <row r="39" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <v>26</v>
       </c>
@@ -5382,7 +5303,7 @@
       <c r="CT39" s="6"/>
       <c r="CU39" s="6"/>
     </row>
-    <row r="40" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
         <v>27</v>
       </c>
@@ -5452,7 +5373,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>28</v>
       </c>
@@ -5522,7 +5443,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="19">
         <v>29</v>
       </c>
@@ -5592,7 +5513,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19">
         <v>30</v>
       </c>
@@ -5722,7 +5643,7 @@
       <c r="CT43" s="6"/>
       <c r="CU43" s="6"/>
     </row>
-    <row r="44" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="19">
         <v>31</v>
       </c>
@@ -5852,7 +5773,7 @@
       <c r="CT44" s="6"/>
       <c r="CU44" s="6"/>
     </row>
-    <row r="45" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>32</v>
       </c>
@@ -5982,7 +5903,7 @@
       <c r="CT45" s="6"/>
       <c r="CU45" s="6"/>
     </row>
-    <row r="46" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19">
         <v>33</v>
       </c>
@@ -6112,7 +6033,7 @@
       <c r="CT46" s="6"/>
       <c r="CU46" s="6"/>
     </row>
-    <row r="47" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19">
         <v>34</v>
       </c>
@@ -6242,7 +6163,7 @@
       <c r="CT47" s="6"/>
       <c r="CU47" s="6"/>
     </row>
-    <row r="48" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
         <v>35</v>
       </c>
@@ -6372,7 +6293,7 @@
       <c r="CT48" s="6"/>
       <c r="CU48" s="6"/>
     </row>
-    <row r="49" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:99" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>36</v>
       </c>
@@ -6502,7 +6423,7 @@
       <c r="CT49" s="6"/>
       <c r="CU49" s="6"/>
     </row>
-    <row r="50" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
         <v>0</v>
       </c>
@@ -6648,7 +6569,7 @@
       </c>
       <c r="AM50" s="66"/>
     </row>
-    <row r="51" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:99" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="20"/>
       <c r="B51" s="21" t="s">
         <v>3</v>
@@ -6792,7 +6713,7 @@
       </c>
       <c r="AM51" s="66"/>
     </row>
-    <row r="52" spans="1:99" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:99" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -6825,7 +6746,7 @@
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
     </row>
-    <row r="120" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="120" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G120" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -6891,7 +6812,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="121" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="121" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G121" t="str">
         <f>IF(AND(G15="x",$AM15="s"),"x","")</f>
         <v/>
@@ -6957,7 +6878,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="122" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G122" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -7023,7 +6944,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="123" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="123" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G123" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -7089,7 +7010,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="124" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="124" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G124" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -7155,7 +7076,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="125" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="125" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G125" t="str">
         <f>IF(AND(G21="x",$AM21="s"),"x","")</f>
         <v/>
@@ -7221,7 +7142,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="126" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G126" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -7287,7 +7208,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="127" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="127" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G127" t="str">
         <f t="shared" ref="G127:I129" si="25">IF(AND(G23="x",$AM23="s"),"x","")</f>
         <v/>
@@ -7353,7 +7274,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="128" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G128" t="str">
         <f t="shared" si="25"/>
         <v/>
@@ -7419,7 +7340,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="129" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G129" t="str">
         <f t="shared" si="25"/>
         <v/>
@@ -7485,7 +7406,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="130" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G130" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -7551,7 +7472,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="131" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="131" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G131" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -7617,7 +7538,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="132" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="132" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>5</v>
       </c>
@@ -7686,7 +7607,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="133" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="133" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G133" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -7752,7 +7673,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="134" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="134" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G134" t="str">
         <f>IF(AND(G26="x",$AM26="s"),"x","")</f>
         <v/>
@@ -7818,7 +7739,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="135" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G135" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -7884,7 +7805,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="136" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="136" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G136" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -7950,7 +7871,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="137" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="137" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G137" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -8016,7 +7937,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="138" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="138" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G138" t="str">
         <f t="shared" ref="G138:I139" si="31">IF(AND(G28="x",$AM28="s"),"x","")</f>
         <v/>
@@ -8082,7 +8003,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="139" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G139" t="str">
         <f t="shared" si="31"/>
         <v/>
@@ -8148,7 +8069,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="140" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G140" t="str">
         <f>IF(AND(G32="x",$AM32="s"),"x","")</f>
         <v/>
@@ -8214,7 +8135,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="141" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G141" t="str">
         <f>IF(AND(G40="x",$AM40="s"),"x","")</f>
         <v/>
@@ -8280,7 +8201,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="142" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G142" t="str">
         <f t="shared" ref="G142:I145" si="36">IF(AND(G43="x",$AM43="s"),"x","")</f>
         <v/>
@@ -8346,7 +8267,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="143" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G143" t="str">
         <f t="shared" si="36"/>
         <v/>
@@ -8412,7 +8333,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="144" spans="2:26" x14ac:dyDescent="0.25">
       <c r="G144" t="str">
         <f t="shared" si="36"/>
         <v/>
@@ -8478,7 +8399,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="145" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G145" t="str">
         <f t="shared" si="36"/>
         <v/>
@@ -8544,7 +8465,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="146" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G146" t="str">
         <f>IF(AND(G49="x",$AM49="s"),"x","")</f>
         <v/>
@@ -8610,7 +8531,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="147" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G147" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -8676,7 +8597,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="148" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="148" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G148" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -8742,7 +8663,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="149" spans="7:26" x14ac:dyDescent="0.15">
+    <row r="149" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G149" t="e">
         <f>IF(AND(#REF!="x",#REF!="s"),"x","")</f>
         <v>#REF!</v>
@@ -8810,26 +8731,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="AE13:AH13"/>
-    <mergeCell ref="AI13:AL13"/>
-    <mergeCell ref="AE12:AL12"/>
-    <mergeCell ref="AD4:AD9"/>
-    <mergeCell ref="AC4:AC9"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="Q4:Q9"/>
-    <mergeCell ref="R4:R9"/>
-    <mergeCell ref="AB4:AB9"/>
-    <mergeCell ref="AA4:AA9"/>
-    <mergeCell ref="Z4:Z9"/>
-    <mergeCell ref="T4:T9"/>
-    <mergeCell ref="W4:W9"/>
-    <mergeCell ref="X4:X9"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F4:F9"/>
-    <mergeCell ref="G4:G9"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C4:E4"/>
     <mergeCell ref="A10:E12"/>
     <mergeCell ref="Y4:Y9"/>
     <mergeCell ref="V4:V9"/>
@@ -8844,13 +8745,32 @@
     <mergeCell ref="H4:H9"/>
     <mergeCell ref="L4:L9"/>
     <mergeCell ref="K4:K9"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="G4:G9"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="Q4:Q9"/>
+    <mergeCell ref="R4:R9"/>
+    <mergeCell ref="AB4:AB9"/>
+    <mergeCell ref="AA4:AA9"/>
+    <mergeCell ref="Z4:Z9"/>
+    <mergeCell ref="T4:T9"/>
+    <mergeCell ref="W4:W9"/>
+    <mergeCell ref="X4:X9"/>
+    <mergeCell ref="AE13:AH13"/>
+    <mergeCell ref="AI13:AL13"/>
+    <mergeCell ref="AE12:AL12"/>
+    <mergeCell ref="AD4:AD9"/>
+    <mergeCell ref="AC4:AC9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" horizontalDpi="360" verticalDpi="360"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>